<commit_message>
Update simulation case 29 files
</commit_message>
<xml_diff>
--- a/SimulationStudyData/Model5/SimCase29_Zsim_SimRun1.xlsx
+++ b/SimulationStudyData/Model5/SimCase29_Zsim_SimRun1.xlsx
@@ -407,34 +407,34 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -463,10 +463,10 @@
         <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -576,22 +576,22 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -599,51 +599,51 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -663,34 +663,34 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -736,16 +736,16 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -797,28 +797,28 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -832,25 +832,25 @@
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -864,25 +864,25 @@
         <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -890,31 +890,31 @@
         <v>2</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -951,34 +951,34 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -998,19 +998,19 @@
         <v>2</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1065,16 +1065,16 @@
         <v>2</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1114,57 +1114,57 @@
         <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -1175,34 +1175,34 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1245,25 +1245,25 @@
         <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1286,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
@@ -1312,89 +1312,89 @@
         <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1414,36 +1414,36 @@
         <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1466,25 +1466,25 @@
         <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="n">
         <v>1</v>
@@ -1551,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" t="n">
         <v>2</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
@@ -1655,34 +1655,34 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1690,16 +1690,16 @@
         <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1722,19 +1722,19 @@
         <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -1783,130 +1783,130 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -1917,28 +1917,28 @@
         <v>2</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1952,25 +1952,25 @@
         <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -2039,66 +2039,66 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2135,22 +2135,22 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G56" t="n">
         <v>2</v>
@@ -2223,15 +2223,15 @@
         <v>2</v>
       </c>
       <c r="I58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B59" t="n">
         <v>2</v>
@@ -2281,16 +2281,16 @@
         <v>2</v>
       </c>
       <c r="G60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2368,48 +2368,48 @@
         <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
         <v>1</v>
@@ -2487,19 +2487,19 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>1</v>
@@ -2534,19 +2534,19 @@
         <v>2</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2615,34 +2615,34 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2662,19 +2662,19 @@
         <v>2</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -2711,42 +2711,42 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" t="n">
         <v>1</v>
@@ -2775,98 +2775,98 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -2921,16 +2921,16 @@
         <v>2</v>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -2985,48 +2985,48 @@
         <v>2</v>
       </c>
       <c r="G82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3040,25 +3040,25 @@
         <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -3075,86 +3075,86 @@
         <v>2</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>2</v>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
@@ -3180,13 +3180,13 @@
         <v>2</v>
       </c>
       <c r="H88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3197,48 +3197,48 @@
         <v>2</v>
       </c>
       <c r="C89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G90" t="n">
         <v>1</v>
@@ -3255,77 +3255,77 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="n">
         <v>2</v>
@@ -3383,13 +3383,13 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="n">
         <v>1</v>
@@ -3415,31 +3415,31 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J96" t="n">
         <v>2</v>
@@ -3456,16 +3456,16 @@
         <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H97" t="n">
         <v>1</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B98" t="n">
         <v>1</v>
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="J98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -3520,25 +3520,25 @@
         <v>2</v>
       </c>
       <c r="D99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -3575,34 +3575,34 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -3642,19 +3642,19 @@
         <v>2</v>
       </c>
       <c r="B103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
@@ -3677,60 +3677,60 @@
         <v>2</v>
       </c>
       <c r="C104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -3753,48 +3753,48 @@
         <v>2</v>
       </c>
       <c r="G106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -3811,7 +3811,7 @@
         <v>2</v>
       </c>
       <c r="E108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F108" t="n">
         <v>1</v>
@@ -3843,13 +3843,13 @@
         <v>2</v>
       </c>
       <c r="E109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H109" t="n">
         <v>1</v>
@@ -3913,21 +3913,21 @@
         <v>2</v>
       </c>
       <c r="G111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B112" t="n">
         <v>1</v>
@@ -3991,66 +3991,66 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -4087,7 +4087,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B117" t="n">
         <v>1</v>
@@ -4114,33 +4114,33 @@
         <v>1</v>
       </c>
       <c r="J117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I118" t="n">
         <v>1</v>
@@ -4151,60 +4151,60 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I120" t="n">
         <v>2</v>
@@ -4279,34 +4279,34 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
@@ -4346,54 +4346,54 @@
         <v>2</v>
       </c>
       <c r="B125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H126" t="n">
         <v>1</v>
@@ -4439,66 +4439,66 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
@@ -4535,34 +4535,34 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -4594,7 +4594,7 @@
         <v>2</v>
       </c>
       <c r="J132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -4663,10 +4663,10 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135" t="n">
         <v>1</v>
@@ -4727,34 +4727,34 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -4768,22 +4768,22 @@
         <v>2</v>
       </c>
       <c r="D138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J138" t="n">
         <v>1</v>
@@ -4791,7 +4791,7 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B139" t="n">
         <v>1</v>
@@ -4823,34 +4823,34 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
@@ -4887,19 +4887,19 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142" t="n">
         <v>2</v>
       </c>
       <c r="D142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F142" t="n">
         <v>1</v>
@@ -4934,19 +4934,19 @@
         <v>2</v>
       </c>
       <c r="F143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -4957,13 +4957,13 @@
         <v>2</v>
       </c>
       <c r="C144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F144" t="n">
         <v>1</v>
@@ -4972,10 +4972,10 @@
         <v>1</v>
       </c>
       <c r="H144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J144" t="n">
         <v>1</v>
@@ -5042,103 +5042,103 @@
         <v>2</v>
       </c>
       <c r="J146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -5187,22 +5187,22 @@
         <v>2</v>
       </c>
       <c r="E151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -5271,25 +5271,25 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H154" t="n">
         <v>1</v>
@@ -5303,34 +5303,34 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -5347,54 +5347,54 @@
         <v>2</v>
       </c>
       <c r="E156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -5405,19 +5405,19 @@
         <v>2</v>
       </c>
       <c r="C158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H158" t="n">
         <v>1</v>
@@ -5431,22 +5431,22 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G159" t="n">
         <v>2</v>
@@ -5463,13 +5463,13 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C160" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D160" t="n">
         <v>2</v>
@@ -5495,7 +5495,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B161" t="n">
         <v>1</v>
@@ -5507,7 +5507,7 @@
         <v>1</v>
       </c>
       <c r="E161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F161" t="n">
         <v>2</v>
@@ -5527,106 +5527,106 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C165" t="n">
         <v>1</v>
@@ -5655,66 +5655,66 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -5772,109 +5772,109 @@
         <v>2</v>
       </c>
       <c r="H169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -5920,13 +5920,13 @@
         <v>2</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G174" t="n">
         <v>1</v>
@@ -5943,19 +5943,19 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E175" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F175" t="n">
         <v>1</v>
@@ -6007,7 +6007,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B177" t="n">
         <v>1</v>
@@ -6039,19 +6039,19 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F178" t="n">
         <v>1</v>
@@ -6071,7 +6071,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B179" t="n">
         <v>1</v>
@@ -6103,34 +6103,34 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -6275,22 +6275,22 @@
         <v>1</v>
       </c>
       <c r="E185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -6322,71 +6322,71 @@
         <v>2</v>
       </c>
       <c r="J186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
@@ -6403,22 +6403,22 @@
         <v>2</v>
       </c>
       <c r="E189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -6429,39 +6429,39 @@
         <v>2</v>
       </c>
       <c r="C190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D191" t="n">
         <v>1</v>
@@ -6519,13 +6519,13 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D193" t="n">
         <v>1</v>
@@ -6540,13 +6540,13 @@
         <v>1</v>
       </c>
       <c r="H193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -6583,31 +6583,31 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J195" t="n">
         <v>1</v>
@@ -6665,30 +6665,30 @@
         <v>1</v>
       </c>
       <c r="G197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E198" t="n">
         <v>1</v>
@@ -6711,77 +6711,77 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D201" t="n">
         <v>1</v>

</xml_diff>